<commit_message>
New forms with PCD form
</commit_message>
<xml_diff>
--- a/xls/COST_Follow_Up.xlsx
+++ b/xls/COST_Follow_Up.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eldo Elobolobo\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13170"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="305">
   <si>
     <t>type</t>
   </si>
@@ -108,26 +113,6 @@
     <t>family_id</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1. N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>úmero do agregado</t>
-    </r>
-  </si>
-  <si>
     <t>formato XXX-XXXX-XXX</t>
   </si>
   <si>
@@ -152,9 +137,6 @@
     <t>dob</t>
   </si>
   <si>
-    <t>2. Data de nascimento</t>
-  </si>
-  <si>
     <t>. &lt;=  today()</t>
   </si>
   <si>
@@ -164,13 +146,7 @@
     <t>gender</t>
   </si>
   <si>
-    <t>3. Sexo</t>
-  </si>
-  <si>
     <t>visit_date</t>
-  </si>
-  <si>
-    <t>4. Data da visita</t>
   </si>
   <si>
     <t>. &lt;=  today() and (. &gt;= date('2016-12-01'))</t>
@@ -182,33 +158,10 @@
     <t>consent</t>
   </si>
   <si>
-    <t>5. Retirou o consentimento de participação?</t>
-  </si>
-  <si>
     <t>Se sim, parar de preencher o inquerito!</t>
   </si>
   <si>
     <t>consent_why</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>6. Se sim</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>, porquê? Especifique</t>
-    </r>
   </si>
   <si>
     <t>${consent} = 1</t>
@@ -238,30 +191,7 @@
     <t>paint</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>7. Reboucou ou pintou a sua casa no ultimo m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ês?</t>
-    </r>
-  </si>
-  <si>
     <t>net_sleepun</t>
-  </si>
-  <si>
-    <t>8. O participante dormiu debaixo da rede mosquiteira?</t>
   </si>
   <si>
     <t>txt</t>
@@ -273,9 +203,6 @@
     <t>net_hole</t>
   </si>
   <si>
-    <t>9. Observe a rede por todos os lados. Tem furos maiores do que a ponta do seu polegar?</t>
-  </si>
-  <si>
     <t>${net_sleepun} = 1</t>
   </si>
   <si>
@@ -285,48 +212,13 @@
     <t>net_loc</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10. Onde est</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>á</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> a rede?</t>
-    </r>
-  </si>
-  <si>
     <t>net_wash</t>
-  </si>
-  <si>
-    <t>11. Lavou a rede desde a minha ultima visita?</t>
   </si>
   <si>
     <t>select_one netwash</t>
   </si>
   <si>
     <t>washnr</t>
-  </si>
-  <si>
-    <t>12. Se sim, quantas vezes?</t>
   </si>
   <si>
     <t>${net_wash} = 1</t>
@@ -338,33 +230,10 @@
     <t>precaution</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">13. Usou algumas das seguintes medidas durante a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>última semana?</t>
-    </r>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
     <t>precaution_cost</t>
-  </si>
-  <si>
-    <t>14. Se sim, quanto pagou?</t>
   </si>
   <si>
     <t>Preenche com "000" se foi gratis</t>
@@ -386,9 +255,6 @@
   </si>
   <si>
     <t>perm_id</t>
-  </si>
-  <si>
-    <t>15. Numero do participante</t>
   </si>
   <si>
     <t>had_malaria</t>
@@ -1027,9 +893,6 @@
     <t>55. A crianca recebeu antimalaricos nos ultimos 30 dias?</t>
   </si>
   <si>
-    <t>select_one drugs</t>
-  </si>
-  <si>
     <t>drug</t>
   </si>
   <si>
@@ -1403,9 +1266,6 @@
     <t>Noere</t>
   </si>
   <si>
-    <t>Sanagalaza</t>
-  </si>
-  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -1420,18 +1280,78 @@
   <si>
     <t>concat("COST_Follow_Up-",${perm_id})</t>
   </si>
+  <si>
+    <t>Formato Errado! Use o formato: XXX</t>
+  </si>
+  <si>
+    <t>(regex(., '^[0-9][0-9][0-9]$'))</t>
+  </si>
+  <si>
+    <t>2. Número do agregado</t>
+  </si>
+  <si>
+    <t>3. Data de nascimento</t>
+  </si>
+  <si>
+    <t>4. Sexo</t>
+  </si>
+  <si>
+    <t>5. Data da visita</t>
+  </si>
+  <si>
+    <t>6. Retirou o consentimento de participação?</t>
+  </si>
+  <si>
+    <t>7. Se sim, porquê? Especifique</t>
+  </si>
+  <si>
+    <t>8. Reboucou ou pintou a sua casa no ultimo mês?</t>
+  </si>
+  <si>
+    <t>9. O participante dormiu debaixo da rede mosquiteira?</t>
+  </si>
+  <si>
+    <t>10. Observe a rede por todos os lados. Tem furos maiores do que a ponta do seu polegar?</t>
+  </si>
+  <si>
+    <t>11. Onde está a rede?</t>
+  </si>
+  <si>
+    <t>12. Lavou a rede desde a minha ultima visita?</t>
+  </si>
+  <si>
+    <t>13. Se sim, quantas vezes?</t>
+  </si>
+  <si>
+    <t>14. Usou algumas das seguintes medidas durante a última semana?</t>
+  </si>
+  <si>
+    <t>15. Se sim, quanto pagou?</t>
+  </si>
+  <si>
+    <t>11. Numero do participante</t>
+  </si>
+  <si>
+    <t>Use o Formato XXX-XXXX-XXX-XXXX</t>
+  </si>
+  <si>
+    <t>(regex(., '^[0-9][0-9][0-9]-[0-9][0-9][0-9][0-9]-[0-9][0-9][0-9]-[0-9][0-9][0-9][0-9]$'))</t>
+  </si>
+  <si>
+    <t>${had_malaria} = 1</t>
+  </si>
+  <si>
+    <t>Sangalaza</t>
+  </si>
+  <si>
+    <t>select_multiple drugs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1450,7 +1370,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1458,152 +1377,8 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1612,13 +1387,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.6"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.25"/>
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1634,182 +1409,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1817,251 +1418,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2151,58 +1510,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2211,7 +1531,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="221F1E"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -2463,32 +1783,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
-      <selection/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomRight" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.2866666666667" style="11" customWidth="1"/>
-    <col min="2" max="2" width="16.3" style="10" customWidth="1"/>
-    <col min="3" max="3" width="53.7" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.9" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.2866666666667" style="10" customWidth="1"/>
-    <col min="6" max="6" width="11" style="10" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="10" customWidth="1"/>
     <col min="7" max="9" width="9" style="10"/>
-    <col min="10" max="10" width="45.14" style="10" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" style="10" customWidth="1"/>
     <col min="11" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" customHeight="1" spans="1:19">
+    <row r="1" spans="1:16384" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2547,7 +1865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" ht="18" customHeight="1" spans="1:16384">
+    <row r="2" spans="1:16384" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>19</v>
       </c>
@@ -18939,7 +18257,7 @@
       <c r="XFC2" s="14"/>
       <c r="XFD2" s="14"/>
     </row>
-    <row r="3" s="3" customFormat="1" ht="15.75" customHeight="1" spans="1:16384">
+    <row r="3" spans="1:16384" s="3" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -35331,7 +34649,7 @@
       <c r="XFC3" s="14"/>
       <c r="XFD3" s="14"/>
     </row>
-    <row r="4" s="3" customFormat="1" ht="16.5" customHeight="1" spans="1:16384">
+    <row r="4" spans="1:16384" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="A4" s="14" t="s">
         <v>22</v>
       </c>
@@ -51723,7 +51041,7 @@
       <c r="XFC4" s="14"/>
       <c r="XFD4" s="14"/>
     </row>
-    <row r="5" s="4" customFormat="1" ht="17" customHeight="1" spans="1:7">
+    <row r="5" spans="1:16384" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -51733,11 +51051,17 @@
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="E5" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>283</v>
+      </c>
       <c r="G5" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="1" ht="17" customHeight="1" spans="1:7">
+    <row r="6" spans="1:16384" s="4" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -51753,24 +51077,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customHeight="1" spans="1:19">
+    <row r="7" spans="1:16384" ht="15" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>26</v>
@@ -51788,15 +51112,15 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
     </row>
-    <row r="8" s="5" customFormat="1" customHeight="1" spans="1:19">
+    <row r="8" spans="1:16384" s="5" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="C8" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>36</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -51815,20 +51139,20 @@
       <c r="R8" s="18"/>
       <c r="S8" s="18"/>
     </row>
-    <row r="9" customHeight="1" spans="1:19">
+    <row r="9" spans="1:16384" ht="15" customHeight="1">
       <c r="A9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>286</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>26</v>
@@ -51846,15 +51170,15 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" customHeight="1" spans="1:19">
+    <row r="10" spans="1:16384" ht="15" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>287</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -51875,20 +51199,20 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
     </row>
-    <row r="11" customHeight="1" spans="1:19">
+    <row r="11" spans="1:16384" ht="15" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>45</v>
+        <v>288</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>26</v>
@@ -51906,18 +51230,18 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
     </row>
-    <row r="12" customHeight="1" spans="1:19">
+    <row r="12" spans="1:16384" ht="15" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>49</v>
+        <v>289</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -51937,15 +51261,15 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" customHeight="1" spans="1:19">
+    <row r="13" spans="1:16384" ht="15" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>290</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -51956,7 +51280,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -51968,9 +51292,9 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" s="5" customFormat="1" customHeight="1" spans="1:19">
+    <row r="14" spans="1:16384" s="5" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -51991,15 +51315,15 @@
       <c r="R14" s="18"/>
       <c r="S14" s="18"/>
     </row>
-    <row r="15" s="6" customFormat="1" customHeight="1" spans="1:19">
+    <row r="15" spans="1:16384" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -52008,7 +51332,7 @@
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
@@ -52020,15 +51344,15 @@
       <c r="R15" s="21"/>
       <c r="S15" s="21"/>
     </row>
-    <row r="16" s="5" customFormat="1" customHeight="1" spans="1:19">
+    <row r="16" spans="1:16384" s="5" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
@@ -52047,15 +51371,15 @@
       <c r="R16" s="18"/>
       <c r="S16" s="18"/>
     </row>
-    <row r="17" customHeight="1" spans="1:19">
+    <row r="17" spans="1:19" ht="15" customHeight="1">
       <c r="A17" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>291</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -52076,15 +51400,15 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" customHeight="1" spans="1:19">
+    <row r="18" spans="1:19" ht="15" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>292</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -52105,15 +51429,15 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" s="7" customFormat="1" customHeight="1" spans="1:19">
+    <row r="19" spans="1:19" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
@@ -52134,15 +51458,15 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" customHeight="1" spans="1:19">
+    <row r="20" spans="1:19" ht="15" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>68</v>
+        <v>293</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -52153,7 +51477,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -52165,15 +51489,15 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
     </row>
-    <row r="21" customHeight="1" spans="1:19">
+    <row r="21" spans="1:19" ht="15" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>294</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -52183,7 +51507,9 @@
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="J21" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -52194,15 +51520,15 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" customHeight="1" spans="1:19">
+    <row r="22" spans="1:19" ht="15" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>74</v>
+        <v>295</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -52212,7 +51538,9 @@
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -52223,15 +51551,15 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
     </row>
-    <row r="23" customHeight="1" spans="1:19">
+    <row r="23" spans="1:19" ht="15" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>77</v>
+        <v>296</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -52242,7 +51570,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -52254,15 +51582,15 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" customHeight="1" spans="1:19">
+    <row r="24" spans="1:19" ht="15" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>297</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -52272,7 +51600,9 @@
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -52283,22 +51613,22 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
-    <row r="25" customHeight="1" spans="1:19">
+    <row r="25" spans="1:19" ht="15" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>84</v>
+        <v>298</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>26</v>
@@ -52306,7 +51636,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -52318,9 +51648,9 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" s="5" customFormat="1" customHeight="1" spans="1:19">
+    <row r="26" spans="1:19" s="5" customFormat="1" ht="15" customHeight="1">
       <c r="A26" s="17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -52341,15 +51671,15 @@
       <c r="R26" s="18"/>
       <c r="S26" s="18"/>
     </row>
-    <row r="27" s="8" customFormat="1" customHeight="1" spans="1:19">
+    <row r="27" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="27" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
@@ -52368,19 +51698,25 @@
       <c r="R27" s="28"/>
       <c r="S27" s="28"/>
     </row>
-    <row r="28" customHeight="1" spans="1:19">
+    <row r="28" spans="1:19" ht="15" customHeight="1">
       <c r="A28" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+        <v>299</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>300</v>
+      </c>
       <c r="G28" s="4" t="s">
         <v>26</v>
       </c>
@@ -52397,15 +51733,15 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" customHeight="1" spans="1:19">
+    <row r="29" spans="1:19" ht="15" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -52426,15 +51762,15 @@
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" customHeight="1" spans="1:19">
+    <row r="30" spans="1:19" ht="15" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -52444,7 +51780,9 @@
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>302</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -52455,15 +51793,15 @@
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" customHeight="1" spans="1:19">
+    <row r="31" spans="1:19" ht="15" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -52473,7 +51811,9 @@
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="J31" s="4" t="s">
+        <v>302</v>
+      </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -52484,15 +51824,15 @@
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" customHeight="1" spans="1:19">
+    <row r="32" spans="1:19" ht="15" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -52513,20 +51853,20 @@
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
     </row>
-    <row r="33" customHeight="1" spans="1:19">
+    <row r="33" spans="1:19" ht="15" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>26</v>
@@ -52534,7 +51874,7 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -52546,20 +51886,20 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
     </row>
-    <row r="34" customHeight="1" spans="1:19">
+    <row r="34" spans="1:19" ht="15" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>26</v>
@@ -52567,7 +51907,7 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -52579,20 +51919,20 @@
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
     </row>
-    <row r="35" customHeight="1" spans="1:19">
+    <row r="35" spans="1:19" ht="15" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>26</v>
@@ -52600,7 +51940,7 @@
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -52612,20 +51952,20 @@
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
     </row>
-    <row r="36" customHeight="1" spans="1:19">
+    <row r="36" spans="1:19" ht="15" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>26</v>
@@ -52633,7 +51973,7 @@
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -52645,15 +51985,15 @@
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
     </row>
-    <row r="37" customHeight="1" spans="1:19">
+    <row r="37" spans="1:19" ht="15" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -52674,20 +52014,20 @@
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
     </row>
-    <row r="38" customHeight="1" spans="1:19">
+    <row r="38" spans="1:19" ht="15" customHeight="1">
       <c r="A38" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>26</v>
@@ -52695,7 +52035,7 @@
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -52707,20 +52047,20 @@
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
     </row>
-    <row r="39" customHeight="1" spans="1:19">
+    <row r="39" spans="1:19" ht="15" customHeight="1">
       <c r="A39" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>26</v>
@@ -52728,7 +52068,7 @@
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
@@ -52740,20 +52080,20 @@
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
     </row>
-    <row r="40" customHeight="1" spans="1:19">
+    <row r="40" spans="1:19" ht="15" customHeight="1">
       <c r="A40" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>26</v>
@@ -52761,7 +52101,7 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
@@ -52773,15 +52113,15 @@
       <c r="R40" s="4"/>
       <c r="S40" s="4"/>
     </row>
-    <row r="41" customHeight="1" spans="1:19">
+    <row r="41" spans="1:19" ht="15" customHeight="1">
       <c r="A41" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -52802,15 +52142,15 @@
       <c r="R41" s="4"/>
       <c r="S41" s="4"/>
     </row>
-    <row r="42" customHeight="1" spans="1:19">
+    <row r="42" spans="1:19" ht="15" customHeight="1">
       <c r="A42" s="30" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -52821,7 +52161,7 @@
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
@@ -52833,20 +52173,20 @@
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
     </row>
-    <row r="43" customHeight="1" spans="1:19">
+    <row r="43" spans="1:19" ht="15" customHeight="1">
       <c r="A43" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>26</v>
@@ -52854,7 +52194,7 @@
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
@@ -52866,22 +52206,22 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
     </row>
-    <row r="44" customHeight="1" spans="1:19">
+    <row r="44" spans="1:19" ht="15" customHeight="1">
       <c r="A44" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>26</v>
@@ -52889,7 +52229,7 @@
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
@@ -52901,22 +52241,22 @@
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
     </row>
-    <row r="45" customHeight="1" spans="1:19">
+    <row r="45" spans="1:19" ht="15" customHeight="1">
       <c r="A45" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>26</v>
@@ -52924,7 +52264,7 @@
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
@@ -52936,22 +52276,22 @@
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
     </row>
-    <row r="46" customHeight="1" spans="1:19">
+    <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>26</v>
@@ -52959,7 +52299,7 @@
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
@@ -52971,22 +52311,22 @@
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
     </row>
-    <row r="47" customHeight="1" spans="1:19">
+    <row r="47" spans="1:19" ht="15" customHeight="1">
       <c r="A47" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>26</v>
@@ -52994,7 +52334,7 @@
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
@@ -53006,15 +52346,15 @@
       <c r="R47" s="4"/>
       <c r="S47" s="4"/>
     </row>
-    <row r="48" customHeight="1" spans="1:19">
+    <row r="48" spans="1:19" ht="15" customHeight="1">
       <c r="A48" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -53035,18 +52375,18 @@
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
     </row>
-    <row r="49" customHeight="1" spans="1:19">
+    <row r="49" spans="1:20" ht="15" customHeight="1">
       <c r="A49" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -53056,7 +52396,7 @@
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
@@ -53068,18 +52408,18 @@
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
     </row>
-    <row r="50" customHeight="1" spans="1:19">
+    <row r="50" spans="1:20" ht="15" customHeight="1">
       <c r="A50" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -53089,7 +52429,7 @@
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -53101,18 +52441,18 @@
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
     </row>
-    <row r="51" customHeight="1" spans="1:19">
+    <row r="51" spans="1:20" ht="15" customHeight="1">
       <c r="A51" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -53122,7 +52462,7 @@
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -53134,15 +52474,15 @@
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
     </row>
-    <row r="52" customHeight="1" spans="1:19">
+    <row r="52" spans="1:20" ht="15" customHeight="1">
       <c r="A52" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -53153,7 +52493,7 @@
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -53165,15 +52505,15 @@
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
     </row>
-    <row r="53" customHeight="1" spans="1:19">
+    <row r="53" spans="1:20" ht="15" customHeight="1">
       <c r="A53" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -53184,7 +52524,7 @@
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -53196,18 +52536,18 @@
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
     </row>
-    <row r="54" customHeight="1" spans="1:19">
+    <row r="54" spans="1:20" ht="15" customHeight="1">
       <c r="A54" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -53217,7 +52557,7 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -53229,15 +52569,15 @@
       <c r="R54" s="4"/>
       <c r="S54" s="4"/>
     </row>
-    <row r="55" s="7" customFormat="1" customHeight="1" spans="1:19">
+    <row r="55" spans="1:20" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A55" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="25"/>
@@ -53258,18 +52598,18 @@
       <c r="R55" s="25"/>
       <c r="S55" s="25"/>
     </row>
-    <row r="56" customHeight="1" spans="1:19">
+    <row r="56" spans="1:20" ht="15" customHeight="1">
       <c r="A56" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -53289,15 +52629,15 @@
       <c r="R56" s="4"/>
       <c r="S56" s="4"/>
     </row>
-    <row r="57" s="7" customFormat="1" customHeight="1" spans="1:20">
+    <row r="57" spans="1:20" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A57" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D57" s="25"/>
       <c r="E57" s="25"/>
@@ -53319,15 +52659,15 @@
       <c r="S57" s="25"/>
       <c r="T57" s="25"/>
     </row>
-    <row r="58" customHeight="1" spans="1:19">
+    <row r="58" spans="1:20" ht="15" customHeight="1">
       <c r="A58" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -53348,22 +52688,22 @@
       <c r="R58" s="4"/>
       <c r="S58" s="4"/>
     </row>
-    <row r="59" customHeight="1" spans="1:19">
+    <row r="59" spans="1:20" ht="15" customHeight="1">
       <c r="A59" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>26</v>
@@ -53371,7 +52711,7 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
@@ -53383,15 +52723,15 @@
       <c r="R59" s="4"/>
       <c r="S59" s="4"/>
     </row>
-    <row r="60" customHeight="1" spans="1:19">
+    <row r="60" spans="1:20" ht="15" customHeight="1">
       <c r="A60" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -53412,22 +52752,22 @@
       <c r="R60" s="4"/>
       <c r="S60" s="4"/>
     </row>
-    <row r="61" customHeight="1" spans="1:19">
+    <row r="61" spans="1:20" ht="15" customHeight="1">
       <c r="A61" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>26</v>
@@ -53435,7 +52775,7 @@
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -53447,15 +52787,15 @@
       <c r="R61" s="4"/>
       <c r="S61" s="4"/>
     </row>
-    <row r="62" customHeight="1" spans="1:19">
+    <row r="62" spans="1:20" ht="15" customHeight="1">
       <c r="A62" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -53476,22 +52816,22 @@
       <c r="R62" s="4"/>
       <c r="S62" s="4"/>
     </row>
-    <row r="63" customHeight="1" spans="1:19">
+    <row r="63" spans="1:20" ht="15" customHeight="1">
       <c r="A63" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>26</v>
@@ -53499,7 +52839,7 @@
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
@@ -53511,15 +52851,15 @@
       <c r="R63" s="4"/>
       <c r="S63" s="4"/>
     </row>
-    <row r="64" customHeight="1" spans="1:19">
+    <row r="64" spans="1:20" ht="15" customHeight="1">
       <c r="A64" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -53540,22 +52880,22 @@
       <c r="R64" s="4"/>
       <c r="S64" s="4"/>
     </row>
-    <row r="65" customHeight="1" spans="1:19">
+    <row r="65" spans="1:19" ht="15" customHeight="1">
       <c r="A65" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>26</v>
@@ -53563,7 +52903,7 @@
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="J65" s="4" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
@@ -53575,15 +52915,15 @@
       <c r="R65" s="4"/>
       <c r="S65" s="4"/>
     </row>
-    <row r="66" customHeight="1" spans="1:19">
+    <row r="66" spans="1:19" ht="15" customHeight="1">
       <c r="A66" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -53604,22 +52944,22 @@
       <c r="R66" s="4"/>
       <c r="S66" s="4"/>
     </row>
-    <row r="67" customHeight="1" spans="1:19">
+    <row r="67" spans="1:19" ht="15" customHeight="1">
       <c r="A67" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>26</v>
@@ -53627,7 +52967,7 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
@@ -53639,15 +52979,15 @@
       <c r="R67" s="4"/>
       <c r="S67" s="4"/>
     </row>
-    <row r="68" customHeight="1" spans="1:19">
+    <row r="68" spans="1:19" ht="15" customHeight="1">
       <c r="A68" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -53668,22 +53008,22 @@
       <c r="R68" s="4"/>
       <c r="S68" s="4"/>
     </row>
-    <row r="69" customHeight="1" spans="1:19">
+    <row r="69" spans="1:19" ht="15" customHeight="1">
       <c r="A69" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>26</v>
@@ -53691,7 +53031,7 @@
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="J69" s="4" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
@@ -53703,15 +53043,15 @@
       <c r="R69" s="4"/>
       <c r="S69" s="4"/>
     </row>
-    <row r="70" customHeight="1" spans="1:19">
+    <row r="70" spans="1:19" ht="15" customHeight="1">
       <c r="A70" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -53732,22 +53072,22 @@
       <c r="R70" s="4"/>
       <c r="S70" s="4"/>
     </row>
-    <row r="71" customHeight="1" spans="1:19">
+    <row r="71" spans="1:19" ht="15" customHeight="1">
       <c r="A71" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>26</v>
@@ -53755,7 +53095,7 @@
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="J71" s="4" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
@@ -53767,15 +53107,15 @@
       <c r="R71" s="4"/>
       <c r="S71" s="4"/>
     </row>
-    <row r="72" customHeight="1" spans="1:19">
+    <row r="72" spans="1:19" ht="15" customHeight="1">
       <c r="A72" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -53796,22 +53136,22 @@
       <c r="R72" s="4"/>
       <c r="S72" s="4"/>
     </row>
-    <row r="73" customHeight="1" spans="1:19">
+    <row r="73" spans="1:19" ht="15" customHeight="1">
       <c r="A73" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>26</v>
@@ -53819,7 +53159,7 @@
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" s="4" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
@@ -53831,15 +53171,15 @@
       <c r="R73" s="4"/>
       <c r="S73" s="4"/>
     </row>
-    <row r="74" customHeight="1" spans="1:19">
+    <row r="74" spans="1:19" ht="15" customHeight="1">
       <c r="A74" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -53860,22 +53200,22 @@
       <c r="R74" s="4"/>
       <c r="S74" s="4"/>
     </row>
-    <row r="75" customHeight="1" spans="1:19">
+    <row r="75" spans="1:19" ht="15" customHeight="1">
       <c r="A75" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>26</v>
@@ -53883,7 +53223,7 @@
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="J75" s="4" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
@@ -53895,15 +53235,15 @@
       <c r="R75" s="4"/>
       <c r="S75" s="4"/>
     </row>
-    <row r="76" customHeight="1" spans="1:19">
+    <row r="76" spans="1:19" ht="15" customHeight="1">
       <c r="A76" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -53924,20 +53264,20 @@
       <c r="R76" s="4"/>
       <c r="S76" s="4"/>
     </row>
-    <row r="77" customHeight="1" spans="1:19">
+    <row r="77" spans="1:19" ht="15" customHeight="1">
       <c r="A77" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
       <c r="F77" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>26</v>
@@ -53955,9 +53295,9 @@
       <c r="R77" s="4"/>
       <c r="S77" s="4"/>
     </row>
-    <row r="78" s="8" customFormat="1" customHeight="1" spans="1:19">
+    <row r="78" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="A78" s="28" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B78" s="28"/>
       <c r="C78" s="28"/>
@@ -53978,15 +53318,15 @@
       <c r="R78" s="28"/>
       <c r="S78" s="28"/>
     </row>
-    <row r="79" s="9" customFormat="1" customHeight="1" spans="1:19">
+    <row r="79" spans="1:19" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A79" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D79" s="19"/>
       <c r="E79" s="19"/>
@@ -54005,15 +53345,15 @@
       <c r="R79" s="19"/>
       <c r="S79" s="19"/>
     </row>
-    <row r="80" customHeight="1" spans="1:19">
+    <row r="80" spans="1:19" ht="15" customHeight="1">
       <c r="A80" s="11" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -54034,15 +53374,15 @@
       <c r="R80" s="4"/>
       <c r="S80" s="4"/>
     </row>
-    <row r="81" customHeight="1" spans="1:19">
+    <row r="81" spans="1:19" ht="15" customHeight="1">
       <c r="A81" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -54063,15 +53403,15 @@
       <c r="R81" s="4"/>
       <c r="S81" s="4"/>
     </row>
-    <row r="82" customHeight="1" spans="1:19">
+    <row r="82" spans="1:19" ht="15" customHeight="1">
       <c r="A82" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -54092,18 +53432,18 @@
       <c r="R82" s="4"/>
       <c r="S82" s="4"/>
     </row>
-    <row r="83" customHeight="1" spans="1:19">
+    <row r="83" spans="1:19" ht="15" customHeight="1">
       <c r="A83" s="11" t="s">
-        <v>214</v>
+        <v>304</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
@@ -54113,7 +53453,7 @@
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="J83" s="4" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
@@ -54125,20 +53465,20 @@
       <c r="R83" s="4"/>
       <c r="S83" s="4"/>
     </row>
-    <row r="84" customHeight="1" spans="1:19">
+    <row r="84" spans="1:19" ht="15" customHeight="1">
       <c r="A84" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>26</v>
@@ -54146,7 +53486,7 @@
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
       <c r="J84" s="4" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
@@ -54158,15 +53498,15 @@
       <c r="R84" s="4"/>
       <c r="S84" s="4"/>
     </row>
-    <row r="85" customHeight="1" spans="1:19">
+    <row r="85" spans="1:19" ht="15" customHeight="1">
       <c r="A85" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -54187,9 +53527,9 @@
       <c r="R85" s="4"/>
       <c r="S85" s="4"/>
     </row>
-    <row r="86" s="9" customFormat="1" customHeight="1" spans="1:19">
+    <row r="86" spans="1:19" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A86" s="33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
@@ -54210,15 +53550,15 @@
       <c r="R86" s="19"/>
       <c r="S86" s="19"/>
     </row>
-    <row r="87" s="9" customFormat="1" customHeight="1" spans="1:19">
+    <row r="87" spans="1:19" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A87" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="D87" s="19"/>
       <c r="E87" s="19"/>
@@ -54237,15 +53577,15 @@
       <c r="R87" s="19"/>
       <c r="S87" s="19"/>
     </row>
-    <row r="88" customHeight="1" spans="1:19">
+    <row r="88" spans="1:19" ht="15" customHeight="1">
       <c r="A88" s="11" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -54266,15 +53606,15 @@
       <c r="R88" s="4"/>
       <c r="S88" s="4"/>
     </row>
-    <row r="89" customHeight="1" spans="1:19">
+    <row r="89" spans="1:19" ht="15" customHeight="1">
       <c r="A89" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -54285,7 +53625,7 @@
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="J89" s="4" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
@@ -54297,15 +53637,15 @@
       <c r="R89" s="4"/>
       <c r="S89" s="4"/>
     </row>
-    <row r="90" customHeight="1" spans="1:19">
+    <row r="90" spans="1:19" ht="15" customHeight="1">
       <c r="A90" s="11" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -54316,7 +53656,7 @@
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="J90" s="4" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
@@ -54328,15 +53668,15 @@
       <c r="R90" s="4"/>
       <c r="S90" s="4"/>
     </row>
-    <row r="91" customHeight="1" spans="1:19">
+    <row r="91" spans="1:19" ht="15" customHeight="1">
       <c r="A91" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -54347,7 +53687,7 @@
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="J91" s="4" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
@@ -54359,9 +53699,9 @@
       <c r="R91" s="4"/>
       <c r="S91" s="4"/>
     </row>
-    <row r="92" s="9" customFormat="1" customHeight="1" spans="1:19">
+    <row r="92" spans="1:19" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A92" s="33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B92" s="19"/>
       <c r="C92" s="19"/>
@@ -54382,9 +53722,9 @@
       <c r="R92" s="19"/>
       <c r="S92" s="19"/>
     </row>
-    <row r="93" s="6" customFormat="1" customHeight="1" spans="1:19">
+    <row r="93" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A93" s="20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="21"/>
@@ -54405,15 +53745,15 @@
       <c r="R93" s="21"/>
       <c r="S93" s="21"/>
     </row>
-    <row r="94" s="10" customFormat="1" customHeight="1" spans="1:19">
+    <row r="94" spans="1:19" ht="15" customHeight="1">
       <c r="A94" s="11" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -54435,36 +53775,33 @@
       <c r="S94" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C3"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.2866666666667" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="3" width="30.4266666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.8533333333333" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:5">
+    <row r="1" spans="1:5" ht="18.95" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -54479,141 +53816,141 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:3">
+    <row r="2" spans="1:5" ht="18.95" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:3">
+    <row r="3" spans="1:5" ht="18.95" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:3">
+    <row r="4" spans="1:5" ht="18.95" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="1:3">
+    <row r="5" spans="1:5" ht="18.95" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="6" customHeight="1" spans="1:3">
+    <row r="6" spans="1:5" ht="18.95" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="7" customHeight="1" spans="1:3">
+    <row r="7" spans="1:5" ht="18.95" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="1:3">
+    <row r="8" spans="1:5" ht="18.95" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B8" s="2">
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="9" customHeight="1" spans="1:3">
+    <row r="9" spans="1:5" ht="18.95" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
-    <row r="10" customHeight="1" spans="1:3">
+    <row r="10" spans="1:5" ht="18.95" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
     </row>
-    <row r="11" customHeight="1" spans="1:3">
+    <row r="11" spans="1:5" ht="18.95" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="1:3">
+    <row r="12" spans="1:5" ht="18.95" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
-    <row r="13" customHeight="1" spans="1:3">
+    <row r="13" spans="1:5" ht="18.95" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B13" s="2">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="14" customHeight="1" spans="1:3">
+    <row r="14" spans="1:5" ht="18.95" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -54622,9 +53959,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="1:3">
+    <row r="15" spans="1:5" ht="18.95" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -54633,9 +53970,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="1:3">
+    <row r="16" spans="1:5" ht="18.95" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
@@ -54644,483 +53981,480 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="1:3">
+    <row r="17" spans="1:3" ht="18.95" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="1:3">
+    <row r="18" spans="1:3" ht="18.95" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B18" s="2">
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="19" customHeight="1" spans="1:3">
+    <row r="19" spans="1:3" ht="18.95" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
     </row>
-    <row r="20" customHeight="1" spans="1:3">
+    <row r="20" spans="1:3" ht="18.95" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
-    <row r="21" customHeight="1" spans="1:3">
+    <row r="21" spans="1:3" ht="18.95" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B21" s="2">
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
     </row>
-    <row r="22" customHeight="1" spans="1:3">
+    <row r="22" spans="1:3" ht="18.95" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B22" s="2">
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="1:3">
+    <row r="23" spans="1:3" ht="18.95" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
     </row>
-    <row r="24" customHeight="1" spans="1:3">
+    <row r="24" spans="1:3" ht="18.95" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="B24" s="2">
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
     </row>
-    <row r="25" customHeight="1" spans="1:3">
+    <row r="25" spans="1:3" ht="18.95" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="B25" s="2">
         <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
     </row>
-    <row r="26" customHeight="1" spans="1:3">
+    <row r="26" spans="1:3" ht="18.95" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="B26" s="2">
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="27" customHeight="1" spans="1:3">
+    <row r="27" spans="1:3" ht="18.95" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
     </row>
-    <row r="28" customHeight="1" spans="1:3">
+    <row r="28" spans="1:3" ht="18.95" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="B28" s="2">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
     </row>
-    <row r="29" customHeight="1" spans="1:3">
+    <row r="29" spans="1:3" ht="18.95" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="B29" s="2">
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="1:3">
+    <row r="30" spans="1:3" ht="18.95" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
     </row>
-    <row r="31" customHeight="1" spans="1:3">
+    <row r="31" spans="1:3" ht="18.95" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B31" s="2">
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
-    <row r="32" customHeight="1" spans="1:3">
+    <row r="32" spans="1:3" ht="18.95" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B32" s="2">
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
     </row>
-    <row r="33" customHeight="1" spans="1:3">
+    <row r="33" spans="1:3" ht="18.95" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B33" s="2">
         <v>4</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
     </row>
-    <row r="34" customHeight="1" spans="1:3">
+    <row r="34" spans="1:3" ht="18.95" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B34" s="2">
         <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
     </row>
-    <row r="35" customHeight="1" spans="1:3">
+    <row r="35" spans="1:3" ht="18.95" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B35" s="2">
         <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
-    <row r="36" customHeight="1" spans="1:3">
+    <row r="36" spans="1:3" ht="18.95" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="B36" s="2">
         <v>7</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="37" customHeight="1" spans="1:3">
+    <row r="37" spans="1:3" ht="18.95" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
     </row>
-    <row r="38" customHeight="1" spans="1:3">
+    <row r="38" spans="1:3" ht="18.95" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="B38" s="2">
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
     </row>
-    <row r="39" customHeight="1" spans="1:3">
+    <row r="39" spans="1:3" ht="18.95" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="B39" s="2">
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
     </row>
-    <row r="40" customHeight="1" spans="1:3">
+    <row r="40" spans="1:3" ht="18.95" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="B40" s="2">
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
     </row>
-    <row r="41" customHeight="1" spans="1:3">
+    <row r="41" spans="1:3" ht="18.95" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
-    <row r="42" customHeight="1" spans="1:3">
+    <row r="42" spans="1:3" ht="18.95" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B42" s="2">
         <v>2</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
-    <row r="43" customHeight="1" spans="1:3">
+    <row r="43" spans="1:3" ht="18.95" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B43" s="2">
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="44" customHeight="1" spans="1:3">
+    <row r="44" spans="1:3" ht="18.95" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B44" s="2">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
     </row>
-    <row r="45" customHeight="1" spans="1:3">
+    <row r="45" spans="1:3" ht="18.95" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B45" s="2">
         <v>2</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
     </row>
-    <row r="46" customHeight="1" spans="1:3">
+    <row r="46" spans="1:3" ht="18.95" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B46" s="2">
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
-    <row r="47" customHeight="1" spans="1:3">
+    <row r="47" spans="1:3" ht="18.95" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B47" s="2">
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
     </row>
-    <row r="48" customHeight="1" spans="1:3">
+    <row r="48" spans="1:3" ht="18.95" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B48" s="2">
         <v>5</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
     </row>
-    <row r="49" customHeight="1" spans="1:3">
+    <row r="49" spans="1:3" ht="18.95" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B49" s="2">
         <v>6</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
     </row>
-    <row r="50" customHeight="1" spans="1:3">
+    <row r="50" spans="1:3" ht="18.95" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B50" s="2">
         <v>7</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
     </row>
-    <row r="51" customHeight="1" spans="1:3">
+    <row r="51" spans="1:3" ht="18.95" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B51" s="2">
         <v>8</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
     </row>
-    <row r="52" customHeight="1" spans="1:3">
+    <row r="52" spans="1:3" ht="18.95" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B52" s="2">
         <v>9</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
-    <row r="53" customHeight="1" spans="1:3">
+    <row r="53" spans="1:3" ht="18.95" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B53" s="2">
         <v>10</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
     </row>
-    <row r="54" customHeight="1" spans="1:3">
+    <row r="54" spans="1:3" ht="18.95" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B54" s="2">
         <v>11</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
-    <row r="55" customHeight="1" spans="1:3">
+    <row r="55" spans="1:3" ht="18.95" customHeight="1">
       <c r="A55" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B55" s="2">
         <v>12</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="14.2" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.4266666666667" style="1" customWidth="1"/>
+    <col min="1" max="2" width="14.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:3">
+    <row r="1" spans="1:3" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:3">
+    <row r="2" spans="1:3" ht="18" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>